<commit_message>
addition of parallel and serial testing
</commit_message>
<xml_diff>
--- a/output_tb_triage_comparison_table.xlsx
+++ b/output_tb_triage_comparison_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,78 +466,104 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>VOC Model (TPP Threshold)</t>
+          <t>Combined Youden's J Optimized with CXR (Parallel)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>93.8</v>
+        <v>94</v>
       </c>
       <c r="C3" t="n">
-        <v>46.7</v>
+        <v>76.5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>VOC Model (Optimized)</t>
+          <t>VOC Model (TPP Optimized)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>75</v>
+        <v>84.40000000000001</v>
       </c>
       <c r="C4" t="n">
-        <v>93.3</v>
+        <v>66.7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CXR + CAD</t>
+          <t>VOC Model (Sensitivity Optimized)</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>90</v>
+        <v>93.8</v>
       </c>
       <c r="C5" t="n">
-        <v>74</v>
+        <v>46.7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CXR</t>
+          <t>VOC Model (Youden's J)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" t="n">
-        <v>82</v>
+        <v>93.3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CRP</t>
+          <t>CXR + CAD</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C7" t="n">
-        <v>61</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>CXR</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>76</v>
+      </c>
+      <c r="C8" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>CRP</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>84</v>
+      </c>
+      <c r="C9" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>Urine LAM</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B10" t="n">
         <v>42</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C10" t="n">
         <v>99</v>
       </c>
     </row>

</xml_diff>